<commit_message>
wednesday, finally the geomaps :)
</commit_message>
<xml_diff>
--- a/Data/Raw/WHY_CORRELATIONS/Employment-regionaldaten-2019-erwerbstaetige.xlsx
+++ b/Data/Raw/WHY_CORRELATIONS/Employment-regionaldaten-2019-erwerbstaetige.xlsx
@@ -5,26 +5,27 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianvaleria/Ironhack/Week_5/Mid_bootcamp_project/DATASETS/B_WHY/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristianvaleria/Ironhack/Week_5/Mid_bootcamp_project/Data/Raw/WHY_CORRELATIONS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCC016D-8E93-F845-B290-0731A8032CD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B789A75E-6475-774C-8E5D-EAC3305C6DCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="10400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="1380" windowWidth="24440" windowHeight="14120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="9" r:id="rId1"/>
+    <sheet name="Employment" sheetId="10" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_AMO_UniqueIdentifier" hidden="1">"'5318fd21-4de5-4b52-9604-7629f5813a7c'"</definedName>
     <definedName name="TABLE" localSheetId="0">Daten!$B$4:$E$39</definedName>
   </definedNames>
-  <calcPr calcId="145621" fullPrecision="0"/>
+  <calcPr calcId="191029" fullPrecision="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Berlin</t>
   </si>
@@ -221,16 +222,23 @@
     <t>Acquisition-
 Employment rate¹</t>
   </si>
+  <si>
+    <t>ID Disctrict</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -309,6 +317,12 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -438,13 +452,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -529,12 +544,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -556,6 +574,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -565,17 +586,26 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Millares [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -924,14 +954,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.5" style="3"/>
     <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
@@ -941,52 +971,52 @@
     <col min="9" max="16384" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12.75" customHeight="1">
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="37" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="36.75" customHeight="1">
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="47" t="s">
+    <row r="2" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="43"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="36" t="s">
         <v>56</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>57</v>
       </c>
       <c r="G2" s="16"/>
-      <c r="H2" s="37"/>
-    </row>
-    <row r="3" spans="1:14" ht="13.5" customHeight="1">
-      <c r="B3" s="42"/>
-      <c r="C3" s="44">
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="43"/>
+      <c r="C3" s="46">
         <v>1000</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="17"/>
       <c r="H3" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25" customHeight="1">
+    <row r="4" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="2"/>
@@ -994,20 +1024,20 @@
       <c r="G4" s="12"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:14" ht="14.25" customHeight="1">
+    <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="18"/>
       <c r="H5" s="20"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:14" ht="13">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="48" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1035,8 +1065,8 @@
       <c r="M6"/>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14" ht="13">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1064,8 +1094,8 @@
       <c r="M7"/>
       <c r="N7"/>
     </row>
-    <row r="8" spans="1:14" ht="13">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="48" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1093,8 +1123,8 @@
       <c r="M8"/>
       <c r="N8"/>
     </row>
-    <row r="9" spans="1:14" ht="13">
-      <c r="A9" s="34" t="s">
+    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="48" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1122,8 +1152,8 @@
       <c r="M9"/>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:14" ht="13">
-      <c r="A10" s="34" t="s">
+    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="48" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1151,8 +1181,8 @@
       <c r="M10"/>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:14" ht="13">
-      <c r="A11" s="34" t="s">
+    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A11" s="48" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1180,8 +1210,8 @@
       <c r="M11"/>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" ht="13">
-      <c r="A12" s="34" t="s">
+    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A12" s="48" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1209,8 +1239,8 @@
       <c r="M12"/>
       <c r="N12"/>
     </row>
-    <row r="13" spans="1:14" ht="13">
-      <c r="A13" s="34" t="s">
+    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="48" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1238,8 +1268,8 @@
       <c r="M13"/>
       <c r="N13"/>
     </row>
-    <row r="14" spans="1:14" ht="13">
-      <c r="A14" s="34" t="s">
+    <row r="14" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="48" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1267,8 +1297,8 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="13">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="48" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1296,8 +1326,8 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" ht="13">
-      <c r="A16" s="34" t="s">
+    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="48" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1325,8 +1355,8 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" ht="13">
-      <c r="A17" s="34" t="s">
+    <row r="17" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A17" s="48" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1354,7 +1384,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" ht="24">
+    <row r="18" spans="1:14" ht="24" x14ac:dyDescent="0.15">
       <c r="B18" s="21" t="s">
         <v>33</v>
       </c>
@@ -1380,7 +1410,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" ht="12" customHeight="1">
+    <row r="19" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="8"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -1395,16 +1425,16 @@
       <c r="M19"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" ht="12" customHeight="1">
+    <row r="20" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
       <c r="G20" s="26"/>
       <c r="H20" s="27"/>
       <c r="I20"/>
@@ -1414,8 +1444,8 @@
       <c r="M20"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" ht="13">
-      <c r="A21" s="35">
+    <row r="21" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A21" s="34">
         <v>12051000</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1444,8 +1474,8 @@
       <c r="M21"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" ht="13">
-      <c r="A22" s="35">
+    <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A22" s="34">
         <v>12052000</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1474,8 +1504,8 @@
       <c r="M22"/>
       <c r="N22"/>
     </row>
-    <row r="23" spans="1:14" ht="13">
-      <c r="A23" s="35">
+    <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="34">
         <v>12053000</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1504,8 +1534,8 @@
       <c r="M23"/>
       <c r="N23"/>
     </row>
-    <row r="24" spans="1:14" ht="13">
-      <c r="A24" s="35">
+    <row r="24" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="34">
         <v>12054000</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1534,8 +1564,8 @@
       <c r="M24"/>
       <c r="N24"/>
     </row>
-    <row r="25" spans="1:14" ht="13">
-      <c r="A25" s="35">
+    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="34">
         <v>12060000</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1564,8 +1594,8 @@
       <c r="M25"/>
       <c r="N25"/>
     </row>
-    <row r="26" spans="1:14" ht="13">
-      <c r="A26" s="35">
+    <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A26" s="34">
         <v>12061000</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1594,8 +1624,8 @@
       <c r="M26"/>
       <c r="N26"/>
     </row>
-    <row r="27" spans="1:14" ht="13">
-      <c r="A27" s="35">
+    <row r="27" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="34">
         <v>12062000</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1624,8 +1654,8 @@
       <c r="M27"/>
       <c r="N27"/>
     </row>
-    <row r="28" spans="1:14" ht="13">
-      <c r="A28" s="35">
+    <row r="28" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A28" s="34">
         <v>12063000</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1654,8 +1684,8 @@
       <c r="M28"/>
       <c r="N28"/>
     </row>
-    <row r="29" spans="1:14" ht="13">
-      <c r="A29" s="35">
+    <row r="29" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A29" s="34">
         <v>12064000</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1684,8 +1714,8 @@
       <c r="M29"/>
       <c r="N29"/>
     </row>
-    <row r="30" spans="1:14" ht="13">
-      <c r="A30" s="35">
+    <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A30" s="34">
         <v>12065000</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1714,8 +1744,8 @@
       <c r="M30"/>
       <c r="N30"/>
     </row>
-    <row r="31" spans="1:14" ht="13">
-      <c r="A31" s="35">
+    <row r="31" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A31" s="34">
         <v>12066000</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1744,8 +1774,8 @@
       <c r="M31"/>
       <c r="N31"/>
     </row>
-    <row r="32" spans="1:14" ht="13">
-      <c r="A32" s="35">
+    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A32" s="34">
         <v>12067000</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1774,8 +1804,8 @@
       <c r="M32"/>
       <c r="N32"/>
     </row>
-    <row r="33" spans="1:15" ht="13">
-      <c r="A33" s="35">
+    <row r="33" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+      <c r="A33" s="34">
         <v>12068000</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1804,8 +1834,8 @@
       <c r="M33"/>
       <c r="N33"/>
     </row>
-    <row r="34" spans="1:15" ht="13">
-      <c r="A34" s="35">
+    <row r="34" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+      <c r="A34" s="34">
         <v>12069000</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1834,8 +1864,8 @@
       <c r="M34"/>
       <c r="N34"/>
     </row>
-    <row r="35" spans="1:15" ht="13">
-      <c r="A35" s="35">
+    <row r="35" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+      <c r="A35" s="34">
         <v>12070000</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1865,8 +1895,8 @@
       <c r="N35"/>
       <c r="O35"/>
     </row>
-    <row r="36" spans="1:15" ht="13">
-      <c r="A36" s="35">
+    <row r="36" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+      <c r="A36" s="34">
         <v>12071000</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1896,8 +1926,8 @@
       <c r="N36"/>
       <c r="O36"/>
     </row>
-    <row r="37" spans="1:15" ht="13">
-      <c r="A37" s="35">
+    <row r="37" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+      <c r="A37" s="34">
         <v>12072000</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1927,8 +1957,8 @@
       <c r="N37"/>
       <c r="O37"/>
     </row>
-    <row r="38" spans="1:15" ht="13">
-      <c r="A38" s="35">
+    <row r="38" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+      <c r="A38" s="34">
         <v>12073000</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1958,7 +1988,7 @@
       <c r="N38"/>
       <c r="O38"/>
     </row>
-    <row r="39" spans="1:15" ht="24">
+    <row r="39" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="B39" s="21" t="s">
         <v>35</v>
       </c>
@@ -1986,7 +2016,7 @@
       <c r="N39"/>
       <c r="O39"/>
     </row>
-    <row r="40" spans="1:15" ht="13">
+    <row r="40" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="B40" s="8"/>
       <c r="C40" s="29"/>
       <c r="D40" s="9"/>
@@ -2002,7 +2032,7 @@
       <c r="N40"/>
       <c r="O40"/>
     </row>
-    <row r="41" spans="1:15" s="10" customFormat="1" ht="36">
+    <row r="41" spans="1:15" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="B41" s="22" t="s">
         <v>34</v>
       </c>
@@ -2030,7 +2060,7 @@
       <c r="N41"/>
       <c r="O41"/>
     </row>
-    <row r="42" spans="1:15" ht="13">
+    <row r="42" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="B42" s="4"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
@@ -2040,14 +2070,14 @@
       <c r="H42" s="11"/>
       <c r="I42"/>
     </row>
-    <row r="43" spans="1:15" ht="13">
+    <row r="43" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="B43" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="1:15" ht="13">
+    <row r="44" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="B44" s="23" t="s">
         <v>38</v>
       </c>
@@ -2070,4 +2100,284 @@
     <oddFooter>&amp;C&amp;F</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60C70B7-5202-4F4C-8353-4F331462C45D}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="53">
+        <v>1</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="51">
+        <v>375483</v>
+      </c>
+      <c r="D2" s="51">
+        <v>207808</v>
+      </c>
+      <c r="E2" s="51">
+        <v>13263</v>
+      </c>
+      <c r="F2" s="51">
+        <v>154411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="54">
+        <v>2</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="51">
+        <v>275392</v>
+      </c>
+      <c r="D3" s="51">
+        <v>163522</v>
+      </c>
+      <c r="E3" s="51">
+        <v>10139</v>
+      </c>
+      <c r="F3" s="51">
+        <v>101731</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="53">
+        <v>3</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="51">
+        <v>395050</v>
+      </c>
+      <c r="D4" s="51">
+        <v>230045</v>
+      </c>
+      <c r="E4" s="51">
+        <v>5151</v>
+      </c>
+      <c r="F4" s="51">
+        <v>159854</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="53">
+        <v>4</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="51">
+        <v>317132</v>
+      </c>
+      <c r="D5" s="51">
+        <v>166627</v>
+      </c>
+      <c r="E5" s="51">
+        <v>6289</v>
+      </c>
+      <c r="F5" s="51">
+        <v>144216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="54">
+        <v>5</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="51">
+        <v>237416</v>
+      </c>
+      <c r="D6" s="51">
+        <v>110043</v>
+      </c>
+      <c r="E6" s="51">
+        <v>6695</v>
+      </c>
+      <c r="F6" s="51">
+        <v>120678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="53">
+        <v>6</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="51">
+        <v>289590</v>
+      </c>
+      <c r="D7" s="51">
+        <v>138726</v>
+      </c>
+      <c r="E7" s="51">
+        <v>4456</v>
+      </c>
+      <c r="F7" s="51">
+        <v>146408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="53">
+        <v>7</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="51">
+        <v>340256</v>
+      </c>
+      <c r="D8" s="51">
+        <v>173252</v>
+      </c>
+      <c r="E8" s="51">
+        <v>10949</v>
+      </c>
+      <c r="F8" s="51">
+        <v>156055</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="54">
+        <v>8</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="51">
+        <v>317952</v>
+      </c>
+      <c r="D9" s="51">
+        <v>149762</v>
+      </c>
+      <c r="E9" s="51">
+        <v>16523</v>
+      </c>
+      <c r="F9" s="51">
+        <v>151667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="53">
+        <v>9</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="51">
+        <v>265484</v>
+      </c>
+      <c r="D10" s="51">
+        <v>148391</v>
+      </c>
+      <c r="E10" s="51">
+        <v>5707</v>
+      </c>
+      <c r="F10" s="51">
+        <v>111385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="53">
+        <v>10</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="51">
+        <v>255783</v>
+      </c>
+      <c r="D11" s="51">
+        <v>126721</v>
+      </c>
+      <c r="E11" s="51">
+        <v>7831</v>
+      </c>
+      <c r="F11" s="51">
+        <v>121231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="54">
+        <v>11</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="51">
+        <v>278860</v>
+      </c>
+      <c r="D12" s="51">
+        <v>145114</v>
+      </c>
+      <c r="E12" s="51">
+        <v>8914</v>
+      </c>
+      <c r="F12" s="51">
+        <v>124833</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="53">
+        <v>12</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="51">
+        <v>255661</v>
+      </c>
+      <c r="D13" s="51">
+        <v>108044</v>
+      </c>
+      <c r="E13" s="51">
+        <v>8323</v>
+      </c>
+      <c r="F13" s="51">
+        <v>139294</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>